<commit_message>
First attempt for icluding individual users' data
</commit_message>
<xml_diff>
--- a/test/electricity grid/devices.xlsx
+++ b/test/electricity grid/devices.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>id</t>
   </si>
@@ -38,25 +38,91 @@
     <t>weekly_use_h</t>
   </si>
   <si>
-    <t>nevera</t>
-  </si>
-  <si>
-    <t>bombillos sala</t>
-  </si>
-  <si>
     <t>PC</t>
   </si>
   <si>
-    <t>ducha electrica</t>
-  </si>
-  <si>
     <t>time_per_use_min</t>
   </si>
   <si>
-    <t>microondas</t>
-  </si>
-  <si>
-    <t>modem+wifi</t>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>Equipo Sonido</t>
+  </si>
+  <si>
+    <t>Nevera</t>
+  </si>
+  <si>
+    <t>Iluminación</t>
+  </si>
+  <si>
+    <t>Ducha</t>
+  </si>
+  <si>
+    <t>TV</t>
+  </si>
+  <si>
+    <t>Codificador TV</t>
+  </si>
+  <si>
+    <t>Plancha</t>
+  </si>
+  <si>
+    <t>Lavadora</t>
+  </si>
+  <si>
+    <t>Laptop</t>
+  </si>
+  <si>
+    <t>Cargadores de celular</t>
+  </si>
+  <si>
+    <t>Microondas</t>
+  </si>
+  <si>
+    <t>Licuadora</t>
+  </si>
+  <si>
+    <t>Router</t>
   </si>
 </sst>
 </file>
@@ -417,15 +483,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
   </cols>
@@ -444,18 +510,18 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C2">
-        <v>600</v>
+        <v>120</v>
       </c>
       <c r="D2">
         <v>42</v>
@@ -465,11 +531,11 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
+      <c r="A3" t="s">
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C3">
         <v>30</v>
@@ -482,14 +548,14 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
+      <c r="A4" t="s">
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C4">
-        <v>200</v>
+        <v>3500</v>
       </c>
       <c r="D4">
         <v>28</v>
@@ -499,14 +565,14 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
+      <c r="A5" t="s">
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C5">
-        <v>3600</v>
+        <v>70</v>
       </c>
       <c r="D5">
         <v>3.5</v>
@@ -516,14 +582,14 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
+      <c r="A6" t="s">
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="C6">
-        <v>1250</v>
+        <v>80</v>
       </c>
       <c r="D6">
         <v>6</v>
@@ -533,20 +599,157 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
+      <c r="A7" t="s">
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="C7">
-        <v>20</v>
+        <v>1100</v>
       </c>
       <c r="D7">
         <v>20</v>
       </c>
       <c r="E7">
         <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8">
+        <v>400</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>140</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10">
+        <v>60</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11">
+        <f>6*7</f>
+        <v>42</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12">
+        <v>1250</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13">
+        <v>400</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14">
+        <v>20</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15">
+        <v>50</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>